<commit_message>
improve somewhere in report
</commit_message>
<xml_diff>
--- a/CA3/data/draft1.xlsx
+++ b/CA3/data/draft1.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Workspace\GPLabR\CA3\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{8F5AD831-7CFF-4E1B-8B38-7E6045A90A33}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A72D0EE6-5D12-46AC-9B68-99EC27A484A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{9450D542-5F53-4C9C-B707-B6308AB70B02}"/>
+    <workbookView minimized="1" xWindow="2568" yWindow="420" windowWidth="18900" windowHeight="11844" xr2:uid="{9450D542-5F53-4C9C-B707-B6308AB70B02}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11">
   <si>
     <t>相对误差</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -41,6 +42,30 @@
   </si>
   <si>
     <t>浓度</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>谱线颜色</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黄色</t>
+  </si>
+  <si>
+    <t>绿色</t>
+  </si>
+  <si>
+    <t>蓝色</t>
+  </si>
+  <si>
+    <t>紫色</t>
+  </si>
+  <si>
+    <t>实验值1/nm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>实验值</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -49,9 +74,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="177" formatCode="0.0"/>
+    <numFmt numFmtId="176" formatCode="0.0"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -66,6 +91,12 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="SimSun"/>
+      <charset val="134"/>
     </font>
   </fonts>
   <fills count="2">
@@ -90,7 +121,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -100,11 +131,14 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -420,87 +454,159 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FDD3F21-A7F5-4DA4-BF11-05337E832588}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:L14"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection sqref="A1:C6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="1" max="2" width="11.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.88671875" style="1"/>
+    <col min="2" max="3" width="11.21875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="11" width="8.88671875" style="1"/>
+    <col min="12" max="12" width="12.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="13" max="16384" width="8.88671875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12">
       <c r="A1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
+    <row r="2" spans="1:12" ht="15.6">
+      <c r="A2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="2">
         <v>578.85</v>
       </c>
-      <c r="B2" s="3">
+      <c r="C2" s="3">
         <v>579.1</v>
       </c>
-      <c r="C2" s="4">
-        <f>ABS(A2-B2)/B2</f>
+      <c r="D2" s="4">
+        <f>ABS(B2-C2)/C2</f>
         <v>4.317043688482127E-4</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
+    <row r="3" spans="1:12" ht="15.6">
+      <c r="A3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2">
         <v>576.65</v>
       </c>
-      <c r="B3" s="3">
+      <c r="C3" s="3">
         <v>577</v>
       </c>
-      <c r="C3" s="4">
-        <f t="shared" ref="C3:C6" si="0">ABS(A3-B3)/B3</f>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D6" si="0">ABS(B3-C3)/C3</f>
         <v>6.0658578856156455E-4</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
+    <row r="4" spans="1:12" ht="15.6">
+      <c r="A4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" s="2">
         <v>545.9</v>
       </c>
-      <c r="B4" s="3">
+      <c r="C4" s="3">
         <v>546.1</v>
       </c>
-      <c r="C4" s="4">
+      <c r="D4" s="4">
         <f t="shared" si="0"/>
         <v>3.6623329060619936E-4</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
+      <c r="L4" s="1">
+        <v>1000000000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" ht="15.6">
+      <c r="A5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="2">
         <v>435.59</v>
       </c>
-      <c r="B5" s="3">
+      <c r="C5" s="3">
         <v>435.8</v>
       </c>
-      <c r="C5" s="4">
+      <c r="D5" s="4">
         <f t="shared" si="0"/>
         <v>4.8187241854069841E-4</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
+      <c r="H5" s="1">
+        <v>436.30720922031827</v>
+      </c>
+      <c r="I5" s="1">
+        <v>546.2969403898162</v>
+      </c>
+      <c r="J5" s="1">
+        <v>578.80414613417565</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.6">
+      <c r="A6" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2">
         <v>404.41</v>
       </c>
-      <c r="B6" s="3">
+      <c r="C6" s="3">
         <v>404.7</v>
       </c>
-      <c r="C6" s="4">
+      <c r="D6" s="4">
         <f t="shared" si="0"/>
         <v>7.1658018285140511E-4</v>
+      </c>
+      <c r="H6" s="1">
+        <v>4.3630720922031825E-7</v>
+      </c>
+      <c r="I6" s="1">
+        <v>5.4629694038981619E-7</v>
+      </c>
+      <c r="J6" s="1">
+        <v>5.7880414613417571E-7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12">
+      <c r="B11" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" ht="15.6">
+      <c r="A12" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B12" s="1">
+        <v>436.30720922031827</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" ht="15.6">
+      <c r="A13" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" s="1">
+        <v>546.2969403898162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" ht="15.6">
+      <c r="A14" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="1">
+        <v>578.80414613417565</v>
       </c>
     </row>
   </sheetData>
@@ -513,13 +619,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CC19DB3-C6A3-4048-93DD-505A602919BD}">
   <dimension ref="A1:D17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+    <sheetView topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -533,7 +639,7 @@
         <v>544.58333333333337</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4">
       <c r="A2">
         <v>0.01</v>
       </c>
@@ -547,7 +653,7 @@
         <v>0.17599999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4">
       <c r="A3">
         <v>0.02</v>
       </c>
@@ -561,7 +667,7 @@
         <v>0.48499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4">
       <c r="A4">
         <v>0.04</v>
       </c>
@@ -575,7 +681,7 @@
         <v>0.65300000000000002</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4">
       <c r="A5">
         <v>0.06</v>
       </c>
@@ -589,7 +695,7 @@
         <v>0.89800000000000002</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4">
       <c r="A6">
         <v>0.08</v>
       </c>
@@ -603,7 +709,7 @@
         <v>1.2490000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4">
       <c r="A7">
         <v>0.1</v>
       </c>
@@ -617,7 +723,7 @@
         <v>1.4750000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4">
       <c r="A11">
         <v>507.6</v>
       </c>
@@ -628,7 +734,7 @@
         <v>545.1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4">
       <c r="A12">
         <v>506.4</v>
       </c>
@@ -639,7 +745,7 @@
         <v>544.6</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4">
       <c r="A13">
         <v>506.4</v>
       </c>
@@ -650,7 +756,7 @@
         <v>544.79999999999995</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4">
       <c r="A14">
         <v>506.4</v>
       </c>
@@ -661,7 +767,7 @@
         <v>544.9</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4">
       <c r="A15">
         <v>505.1</v>
       </c>
@@ -672,7 +778,7 @@
         <v>544.29999999999995</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4">
       <c r="A16">
         <v>506</v>
       </c>
@@ -683,7 +789,7 @@
         <v>543.79999999999995</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:3">
       <c r="A17">
         <f>AVERAGE(A11:A16)</f>
         <v>506.31666666666666</v>
@@ -704,4 +810,95 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D603C50D-BC36-4448-9DEC-CE4A96C92D68}">
+  <dimension ref="B1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D8" sqref="D8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8"/>
+  <cols>
+    <col min="2" max="3" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.5546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:4">
+      <c r="B1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="2:4">
+      <c r="B2" s="2">
+        <v>578.85</v>
+      </c>
+      <c r="C2" s="3">
+        <v>579.1</v>
+      </c>
+      <c r="D2" s="4">
+        <f>ABS(B2-C2)/C2</f>
+        <v>4.317043688482127E-4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:4">
+      <c r="B3" s="2">
+        <v>576.65</v>
+      </c>
+      <c r="C3" s="3">
+        <v>577</v>
+      </c>
+      <c r="D3" s="4">
+        <f t="shared" ref="D3:D6" si="0">ABS(B3-C3)/C3</f>
+        <v>6.0658578856156455E-4</v>
+      </c>
+    </row>
+    <row r="4" spans="2:4">
+      <c r="B4" s="2">
+        <v>545.9</v>
+      </c>
+      <c r="C4" s="3">
+        <v>546.1</v>
+      </c>
+      <c r="D4" s="4">
+        <f t="shared" si="0"/>
+        <v>3.6623329060619936E-4</v>
+      </c>
+    </row>
+    <row r="5" spans="2:4">
+      <c r="B5" s="2">
+        <v>435.59</v>
+      </c>
+      <c r="C5" s="3">
+        <v>435.8</v>
+      </c>
+      <c r="D5" s="4">
+        <f t="shared" si="0"/>
+        <v>4.8187241854069841E-4</v>
+      </c>
+    </row>
+    <row r="6" spans="2:4">
+      <c r="B6" s="2">
+        <v>404.41</v>
+      </c>
+      <c r="C6" s="3">
+        <v>404.7</v>
+      </c>
+      <c r="D6" s="4">
+        <f t="shared" si="0"/>
+        <v>7.1658018285140511E-4</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>